<commit_message>
update related C4 figures
</commit_message>
<xml_diff>
--- a/data/sites_info.xlsx
+++ b/data/sites_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiawei/Documents/Work/2023- redclay westerly/RedClay_jet/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geo-checkout-user/Documents/2024_westerly/redclay_jet/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4821DBD1-360C-6745-B8C1-9A8A2AAD53A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7143453B-C0A7-954C-9A1B-D4DE510D9FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="2840" windowWidth="24500" windowHeight="17040" xr2:uid="{0C4DC5BA-BDDE-D944-A995-04B415C2673E}"/>
+    <workbookView xWindow="10060" yWindow="2840" windowWidth="24500" windowHeight="17040" xr2:uid="{0C4DC5BA-BDDE-D944-A995-04B415C2673E}"/>
   </bookViews>
   <sheets>
     <sheet name="site" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
     <t>location</t>
   </si>
@@ -114,6 +114,27 @@
   </si>
   <si>
     <t>Xifeng</t>
+  </si>
+  <si>
+    <t>U1430</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>ODP 1208</t>
+  </si>
+  <si>
+    <t>pacific</t>
+  </si>
+  <si>
+    <t>ODP 885/886</t>
+  </si>
+  <si>
+    <t>Yushe</t>
+  </si>
+  <si>
+    <t>CLP</t>
   </si>
 </sst>
 </file>
@@ -469,318 +490,495 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8496ACD-C802-A84D-BA3B-CA1055DC7FA6}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>38</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>110.5</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>1000</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>19</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>0.19089309282886055</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>433.90000000000003</v>
       </c>
-      <c r="I2" s="1">
+      <c r="K2" s="1">
         <v>10.933333333333332</v>
       </c>
-      <c r="J2" s="1">
+      <c r="L2" s="1">
         <v>25.2</v>
       </c>
-      <c r="K2" s="1">
+      <c r="M2" s="1">
         <v>14.266666666666667</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="C3">
+      <c r="E3">
         <v>36.9</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>110.1</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>1000</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>19</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>0.29396398399288565</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>528.9</v>
       </c>
-      <c r="I3" s="1">
+      <c r="K3" s="1">
         <v>9.9749999999999996</v>
       </c>
-      <c r="J3" s="1">
+      <c r="L3" s="1">
         <v>23.566666666666666</v>
       </c>
-      <c r="K3" s="1">
+      <c r="M3" s="1">
         <v>13.591666666666667</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="C4">
+      <c r="E4">
         <v>34.200000000000003</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>109.3</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>700</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>19</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>0.52216498585213666</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>719.7</v>
       </c>
-      <c r="I4" s="1">
+      <c r="K4" s="1">
         <v>14.6</v>
       </c>
-      <c r="J4" s="1">
+      <c r="L4" s="1">
         <v>27.3</v>
       </c>
-      <c r="K4" s="1">
+      <c r="M4" s="1">
         <v>12.700000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="C5">
+      <c r="E5">
         <v>39.43</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>111.51</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>411.3</v>
       </c>
-      <c r="I5" s="1">
+      <c r="K5" s="1">
         <v>7.4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="C6">
+      <c r="E6">
         <v>35</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>107.58</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>19</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>637.70000000000005</v>
       </c>
-      <c r="I6" s="1">
+      <c r="K6" s="1">
         <v>8.6</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="C7">
+      <c r="E7">
         <v>38.03</v>
       </c>
-      <c r="D7">
+      <c r="F7">
         <v>114.51</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <v>250</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
         <v>24</v>
       </c>
-      <c r="C8">
+      <c r="E8">
         <v>34.25</v>
       </c>
-      <c r="D8">
+      <c r="F8">
         <v>108.95</v>
       </c>
-      <c r="E8">
+      <c r="G8">
         <v>350</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
         <v>24</v>
       </c>
-      <c r="C9">
+      <c r="E9">
         <v>27.72</v>
       </c>
-      <c r="D9">
+      <c r="F9">
         <v>106.92</v>
       </c>
-      <c r="E9">
+      <c r="G9">
         <v>863</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
         <v>24</v>
       </c>
-      <c r="C10">
+      <c r="E10">
         <v>25.27</v>
       </c>
-      <c r="D10">
+      <c r="F10">
         <v>110.28</v>
       </c>
-      <c r="E10">
+      <c r="G10">
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
         <v>15</v>
       </c>
-      <c r="C11">
+      <c r="E11">
         <v>35.74</v>
       </c>
-      <c r="D11">
+      <c r="F11">
         <v>107.66</v>
       </c>
-      <c r="H11">
+      <c r="J11">
         <v>537</v>
       </c>
-      <c r="I11" s="1">
+      <c r="K11" s="1">
         <v>9.4</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
         <v>15</v>
       </c>
-      <c r="C12">
+      <c r="E12">
         <v>38.799999999999997</v>
       </c>
-      <c r="D12">
+      <c r="F12">
         <v>111.2</v>
       </c>
-      <c r="E12">
+      <c r="G12">
         <v>1300</v>
       </c>
-      <c r="F12" t="s">
+      <c r="H12" t="s">
         <v>19</v>
       </c>
-      <c r="G12">
+      <c r="I12">
         <v>0.22842733539999072</v>
       </c>
-      <c r="H12">
+      <c r="J12">
         <v>493.7</v>
       </c>
-      <c r="I12" s="1">
+      <c r="K12" s="1">
         <v>10.175000000000001</v>
       </c>
-      <c r="J12" s="1">
+      <c r="L12" s="1">
         <v>23.433333333333334</v>
       </c>
-      <c r="K12" s="1">
+      <c r="M12" s="1">
         <v>13.258333333333333</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13">
+        <f>37+54.16/60</f>
+        <v>37.902666666666669</v>
+      </c>
+      <c r="F13">
+        <f>131+32.25/60</f>
+        <v>131.53749999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14">
+        <f>38+50/60</f>
+        <v>38.833333333333336</v>
+      </c>
+      <c r="F14">
+        <f>117+26/60</f>
+        <v>117.43333333333334</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="b">
+        <v>1</v>
+      </c>
+      <c r="C15" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <f>36.1</f>
+        <v>36.1</v>
+      </c>
+      <c r="F15">
+        <v>158.19999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="b">
+        <v>1</v>
+      </c>
+      <c r="C16" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16">
+        <v>44.7</v>
+      </c>
+      <c r="F16">
+        <v>-168.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17">
+        <v>37</v>
+      </c>
+      <c r="F17">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>